<commit_message>
included puzzles till latest doa version of markus
</commit_message>
<xml_diff>
--- a/data/Antennas.xlsx
+++ b/data/Antennas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C5F7AA-A58D-41C6-B70A-864849B0B208}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEF7531-681C-448D-9656-B6DA3780EFE5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,21 @@
   </si>
   <si>
     <t>Longitute</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>receiver_1</t>
+  </si>
+  <si>
+    <t>receiver_2</t>
+  </si>
+  <si>
+    <t>receiver_3</t>
+  </si>
+  <si>
+    <t>receiver_4</t>
   </si>
 </sst>
 </file>
@@ -355,15 +370,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -372,6 +391,65 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1.234</v>
+      </c>
+      <c r="C2">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1.234</v>
+      </c>
+      <c r="C3">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1.234</v>
+      </c>
+      <c r="C4">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="D4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>1.234</v>
+      </c>
+      <c r="C5">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="D5">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>